<commit_message>
Correcao pvs placa 04A
</commit_message>
<xml_diff>
--- a/PVs/piso.xlsx
+++ b/PVs/piso.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonardo.leao\Desktop\Concrete-Instrum-Scripts\PVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B62105-BCE2-469E-BC6E-DB673FC924B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C661DA0-1C06-4E80-89FD-49DFD2B5953B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="1785" windowWidth="21600" windowHeight="11400" xr2:uid="{8C664926-5403-41C4-B638-B597EA4F600E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C664926-5403-41C4-B638-B597EA4F600E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="11">
   <si>
     <t>Localização</t>
   </si>
@@ -60,18 +60,6 @@
   </si>
   <si>
     <t>C_V</t>
-  </si>
-  <si>
-    <t>A_Hxyy</t>
-  </si>
-  <si>
-    <t>C_Hxyy</t>
-  </si>
-  <si>
-    <t>A_Hxyx</t>
-  </si>
-  <si>
-    <t>C_Hxyx</t>
   </si>
   <si>
     <t>A_Hxy</t>
@@ -443,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270F984E-E2EF-4600-9BDF-C6DAF7FA9D6F}">
   <dimension ref="A1:D305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,7 +855,7 @@
         <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C30" s="1">
         <v>24</v>
@@ -881,7 +869,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C31" s="1">
         <v>24</v>
@@ -979,7 +967,7 @@
         <v>10</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C38" s="1">
         <v>28</v>
@@ -993,7 +981,7 @@
         <v>10</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C39" s="1">
         <v>28</v>
@@ -1063,7 +1051,7 @@
         <v>13</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C44" s="1">
         <v>28</v>
@@ -1105,7 +1093,7 @@
         <v>13</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C47" s="1">
         <v>28</v>
@@ -1203,7 +1191,7 @@
         <v>16</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C54" s="1">
         <v>29</v>
@@ -1217,7 +1205,7 @@
         <v>16</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C55" s="1">
         <v>29</v>
@@ -1315,7 +1303,7 @@
         <v>20</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C62" s="1">
         <v>29</v>
@@ -1329,7 +1317,7 @@
         <v>20</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C63" s="1">
         <v>29</v>
@@ -1567,7 +1555,7 @@
         <v>7</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C80" s="1">
         <v>17</v>
@@ -1595,7 +1583,7 @@
         <v>7</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C82" s="1">
         <v>17</v>
@@ -1665,7 +1653,7 @@
         <v>4</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C87" s="1">
         <v>15</v>
@@ -1693,7 +1681,7 @@
         <v>4</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C89" s="1">
         <v>15</v>
@@ -1763,7 +1751,7 @@
         <v>3</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C94" s="1">
         <v>15</v>
@@ -1791,7 +1779,7 @@
         <v>3</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C96" s="1">
         <v>15</v>
@@ -1861,7 +1849,7 @@
         <v>6</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C101" s="1">
         <v>16</v>
@@ -1889,7 +1877,7 @@
         <v>6</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C103" s="1">
         <v>16</v>
@@ -1917,7 +1905,7 @@
         <v>1</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C105" s="1">
         <v>16</v>
@@ -1945,7 +1933,7 @@
         <v>1</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C107" s="1">
         <v>16</v>
@@ -1973,7 +1961,7 @@
         <v>9</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C109" s="1">
         <v>16</v>
@@ -2001,7 +1989,7 @@
         <v>9</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C111" s="1">
         <v>16</v>
@@ -2435,7 +2423,7 @@
         <v>7</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C142" s="1">
         <v>3</v>
@@ -2463,7 +2451,7 @@
         <v>7</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C144" s="1">
         <v>3</v>
@@ -2533,7 +2521,7 @@
         <v>4</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C149" s="1">
         <v>3</v>
@@ -2561,7 +2549,7 @@
         <v>4</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C151" s="1">
         <v>4</v>
@@ -2631,7 +2619,7 @@
         <v>3</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C156" s="1">
         <v>4</v>
@@ -2659,7 +2647,7 @@
         <v>3</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C158" s="1">
         <v>4</v>
@@ -2729,7 +2717,7 @@
         <v>6</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C163" s="1">
         <v>4</v>
@@ -2757,7 +2745,7 @@
         <v>6</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C165" s="1">
         <v>4</v>
@@ -2785,7 +2773,7 @@
         <v>1</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C167" s="1">
         <v>5</v>
@@ -2813,7 +2801,7 @@
         <v>1</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C169" s="1">
         <v>5</v>
@@ -2841,7 +2829,7 @@
         <v>9</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C171" s="1">
         <v>5</v>
@@ -2869,7 +2857,7 @@
         <v>9</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C173" s="1">
         <v>5</v>
@@ -3303,7 +3291,7 @@
         <v>7</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C204" s="1">
         <v>7</v>
@@ -3331,7 +3319,7 @@
         <v>7</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C206" s="1">
         <v>7</v>
@@ -3401,7 +3389,7 @@
         <v>4</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C211" s="1">
         <v>7</v>
@@ -3429,7 +3417,7 @@
         <v>4</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C213" s="1">
         <v>8</v>
@@ -3499,7 +3487,7 @@
         <v>3</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C218" s="1">
         <v>8</v>
@@ -3527,7 +3515,7 @@
         <v>3</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C220" s="1">
         <v>8</v>
@@ -3597,7 +3585,7 @@
         <v>6</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C225" s="1">
         <v>8</v>
@@ -3625,7 +3613,7 @@
         <v>6</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C227" s="1">
         <v>8</v>
@@ -3653,7 +3641,7 @@
         <v>1</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C229" s="1">
         <v>9</v>
@@ -3681,7 +3669,7 @@
         <v>1</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C231" s="1">
         <v>9</v>
@@ -3709,7 +3697,7 @@
         <v>9</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C233" s="1">
         <v>9</v>
@@ -3737,7 +3725,7 @@
         <v>9</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C235" s="1">
         <v>9</v>
@@ -4171,7 +4159,7 @@
         <v>7</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C266" s="1">
         <v>11</v>
@@ -4199,7 +4187,7 @@
         <v>7</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C268" s="1">
         <v>11</v>
@@ -4269,7 +4257,7 @@
         <v>4</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C273" s="1">
         <v>11</v>
@@ -4297,7 +4285,7 @@
         <v>4</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C275" s="1">
         <v>12</v>
@@ -4367,7 +4355,7 @@
         <v>3</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C280" s="1">
         <v>12</v>
@@ -4395,7 +4383,7 @@
         <v>3</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C282" s="1">
         <v>12</v>
@@ -4465,7 +4453,7 @@
         <v>6</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C287" s="1">
         <v>12</v>
@@ -4493,7 +4481,7 @@
         <v>6</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C289" s="1">
         <v>12</v>
@@ -4521,7 +4509,7 @@
         <v>1</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C291" s="1">
         <v>13</v>
@@ -4549,7 +4537,7 @@
         <v>1</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C293" s="1">
         <v>13</v>
@@ -4577,7 +4565,7 @@
         <v>9</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C295" s="1">
         <v>13</v>
@@ -4605,7 +4593,7 @@
         <v>9</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C297" s="1">
         <v>13</v>

</xml_diff>